<commit_message>
Login y Register completos
</commit_message>
<xml_diff>
--- a/Requerimientos y versiones.xlsx
+++ b/Requerimientos y versiones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/samir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D11C96C7-6A5C-F74D-BB62-81213ABB38F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D1E833-4E37-654E-BE07-2DBAEE4142DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{B312433B-6778-2443-A57B-6DDFB0A040B1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>#</t>
   </si>
@@ -78,6 +78,9 @@
     <t>0.0.2</t>
   </si>
   <si>
+    <t>0.0.3</t>
+  </si>
+  <si>
     <t>Cargar template metronic - menu lateral - menu top - inicio - footer</t>
   </si>
   <si>
@@ -103,6 +106,12 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hacer Cuenta cliente</t>
+  </si>
+  <si>
+    <t>hacer listado de motores, con orden paginacion, dos vistas</t>
   </si>
 </sst>
 </file>
@@ -124,12 +133,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,9 +159,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +480,7 @@
   <dimension ref="A5:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -497,7 +513,7 @@
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
@@ -511,7 +527,7 @@
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
@@ -525,7 +541,7 @@
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -537,7 +553,7 @@
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
@@ -549,7 +565,7 @@
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
@@ -589,7 +605,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -600,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -611,7 +627,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -622,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
@@ -633,7 +649,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -644,7 +660,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -655,7 +671,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
@@ -666,7 +682,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -676,10 +692,19 @@
       <c r="A21">
         <v>16</v>
       </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>